<commit_message>
Generated the excel file
</commit_message>
<xml_diff>
--- a/results/statistics.xlsx
+++ b/results/statistics.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,16 +470,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7422037422037422</v>
+        <v>0.782051282051282</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7531645569620253</v>
+        <v>0.8</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9807692307692307</v>
+        <v>0.9721115537848606</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8520286396181384</v>
+        <v>0.8776978417266188</v>
       </c>
     </row>
     <row r="3">
@@ -489,54 +489,73 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7477064220183486</v>
+        <v>0.8356060606060606</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7616822429906542</v>
+        <v>0.8452107279693487</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9760479041916168</v>
+        <v>0.9865831842576028</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8556430446194226</v>
+        <v>0.9104416013206768</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Multiplication</t>
+          <t>Common-Divison</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5387596899224806</v>
+        <v>0.875</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5991379310344828</v>
+        <v>0.875</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8424242424242424</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7002518891687657</v>
+        <v>0.9333333333333333</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Multiplication</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7182044887780549</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.9028213166144201</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Subtraction</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>0.6704180064308681</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.6921161825726141</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.9553264604810997</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.8026948989412898</v>
+      <c r="B6" t="n">
+        <v>0.7756591337099812</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.7943587270973963</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.9705449189985272</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.873657695876972</v>
       </c>
     </row>
   </sheetData>
@@ -590,16 +609,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7047146401985112</v>
+        <v>0.7925</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7282051282051282</v>
+        <v>0.8134462406979728</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9562289562289562</v>
+        <v>0.9685304002444241</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8267831149927219</v>
+        <v>0.8842398884239888</v>
       </c>
     </row>
     <row r="3">
@@ -607,16 +626,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6644628099173554</v>
+        <v>0.75775</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6877673224978614</v>
+        <v>0.7789771267026472</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9514792899408284</v>
+        <v>0.9652866242038216</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7984111221449851</v>
+        <v>0.8621817664628076</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +649,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -668,58 +687,77 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>gemini</t>
+          <t>deepseek</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8280166435506241</v>
+        <v>0.914</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8291666666666667</v>
+        <v>0.944702842377261</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9983277591973244</v>
+        <v>0.965662968832541</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9059180576631261</v>
+        <v>0.955067920585162</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>llama3</t>
+          <t>gemini</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4901574803149606</v>
+        <v>0.8555</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5314834578441836</v>
+        <v>0.85678517776665</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8630849220103987</v>
+        <v>0.9982497082847142</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6578599735799208</v>
+        <v>0.9221234168687686</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>llama3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.4915</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.5293484114162628</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8730017761989343</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.659068052296346</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>mistral</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0.8225806451612904</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.8225806451612904</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.9026548672566371</v>
+      <c r="B5" t="n">
+        <v>0.8395</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.83991995997999</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.9994047619047619</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.9127480293558032</v>
       </c>
     </row>
   </sheetData>
@@ -768,13 +806,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="C2" t="n">
-        <v>318</v>
+        <v>727</v>
       </c>
       <c r="D2" t="n">
-        <v>852</v>
+        <v>3170</v>
       </c>
     </row>
     <row r="3">
@@ -782,13 +820,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="C3" t="n">
-        <v>365</v>
+        <v>860</v>
       </c>
       <c r="D3" t="n">
-        <v>804</v>
+        <v>3031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>